<commit_message>
adding Project2 and Project3
</commit_message>
<xml_diff>
--- a/Project1_DataDrivenFramework/src/test/resources/excel/TextData.xlsx
+++ b/Project1_DataDrivenFramework/src/test/resources/excel/TextData.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/namanpatel/Documents/Selenium/Selenium_Projects/Project1_DataDrivenFramework/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF0CC00-AE92-644A-A6E4-FBC338FAB787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F97DA6C3-70B3-3845-902F-18BDFB3A1C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="660" windowWidth="27760" windowHeight="17160" xr2:uid="{7F0AADA6-3404-E045-95AF-5EC468B0C513}"/>
+    <workbookView xWindow="960" yWindow="660" windowWidth="27760" windowHeight="17160" activeTab="2" xr2:uid="{7F0AADA6-3404-E045-95AF-5EC468B0C513}"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
+    <sheet name="Test_Suite" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>FirstName</t>
   </si>
@@ -63,19 +65,82 @@
   </si>
   <si>
     <t>6262AM</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Rupee</t>
+  </si>
+  <si>
+    <t>Dollar</t>
+  </si>
+  <si>
+    <t>TestCase_ID</t>
+  </si>
+  <si>
+    <t>RunMode</t>
+  </si>
+  <si>
+    <t>AddCustomerTest</t>
+  </si>
+  <si>
+    <t>BankManagerLoginTest</t>
+  </si>
+  <si>
+    <t>OpenAccountTest</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Harry Potter</t>
+  </si>
+  <si>
+    <t>Ron Weasly</t>
+  </si>
+  <si>
+    <t>Prince</t>
+  </si>
+  <si>
+    <t>Rai</t>
+  </si>
+  <si>
+    <t>9423PR</t>
+  </si>
+  <si>
+    <t>Akshat</t>
+  </si>
+  <si>
+    <t>Verma</t>
+  </si>
+  <si>
+    <t>7645AV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,8 +163,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,45 +501,183 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D8C2960-F38D-DA4C-ADDE-A693B3DEECD2}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AFBE947-2B8A-9047-B1B5-3352660D3874}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="15.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EEE023C-20E0-EF46-94C8-B933DDDB54DF}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>